<commit_message>
Correct R5 binary reports for existing test data sources
</commit_message>
<xml_diff>
--- a/tests/bin/sample_COUNTER_R5_reports/sample_DR_reports.xlsx
+++ b/tests/bin/sample_COUNTER_R5_reports/sample_DR_reports.xlsx
@@ -722,9 +722,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -754,6 +751,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:W75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1072,373 +1072,373 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="20">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
+      <c r="B12" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="6" t="s">
@@ -4797,6 +4797,12 @@
     </sortState>
   </autoFilter>
   <mergeCells count="13">
+    <mergeCell ref="B6:W6"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="B3:W3"/>
+    <mergeCell ref="B4:W4"/>
+    <mergeCell ref="B5:W5"/>
     <mergeCell ref="B13:W13"/>
     <mergeCell ref="B7:W7"/>
     <mergeCell ref="B8:W8"/>
@@ -4804,12 +4810,6 @@
     <mergeCell ref="B10:W10"/>
     <mergeCell ref="B11:W11"/>
     <mergeCell ref="B12:W12"/>
-    <mergeCell ref="B6:W6"/>
-    <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="B3:W3"/>
-    <mergeCell ref="B4:W4"/>
-    <mergeCell ref="B5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4819,8 +4819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4931,40 +4931,40 @@
       <c r="G14" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>43647</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <v>43678</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <v>43709</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="8">
         <v>43739</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>43770</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="8">
         <v>43800</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="8">
         <v>43831</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="8">
         <v>43862</v>
       </c>
-      <c r="P14" s="9">
+      <c r="P14" s="8">
         <v>43891</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q14" s="8">
         <v>43922</v>
       </c>
-      <c r="R14" s="9">
+      <c r="R14" s="8">
         <v>43952</v>
       </c>
-      <c r="S14" s="9">
+      <c r="S14" s="8">
         <v>43983</v>
       </c>
     </row>
@@ -5764,13 +5764,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1"/>
@@ -5792,160 +5789,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="22.5" customHeight="1">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="86.25" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="M14" s="17" t="s">
+      <c r="M14" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="P14" s="17" t="s">
+      <c r="P14" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="Q14" s="17" t="s">
+      <c r="Q14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="R14" s="17" t="s">
+      <c r="R14" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="S14" s="17" t="s">
+      <c r="S14" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="T14" s="17" t="s">
+      <c r="T14" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="U14" s="17" t="s">
+      <c r="U14" s="16" t="s">
         <v>77</v>
       </c>
     </row>
@@ -5953,62 +5950,62 @@
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="15" t="s">
+      <c r="G15" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="13">
         <v>130</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="12">
         <v>7</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="12">
         <v>9</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="12">
         <v>18</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="12">
         <v>16</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="12">
         <v>16</v>
       </c>
-      <c r="O15" s="13">
-        <v>3</v>
-      </c>
-      <c r="P15" s="13">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="13">
+      <c r="O15" s="12">
+        <v>3</v>
+      </c>
+      <c r="P15" s="12">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="12">
         <v>25</v>
       </c>
-      <c r="R15" s="13">
+      <c r="R15" s="12">
         <v>7</v>
       </c>
-      <c r="S15" s="13">
+      <c r="S15" s="12">
         <v>9</v>
       </c>
-      <c r="T15" s="13">
+      <c r="T15" s="12">
         <v>9</v>
       </c>
-      <c r="U15" s="13">
+      <c r="U15" s="12">
         <v>7</v>
       </c>
     </row>
@@ -6016,62 +6013,62 @@
       <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="G16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <v>29</v>
       </c>
-      <c r="J16" s="10">
-        <v>0</v>
-      </c>
-      <c r="K16" s="10">
-        <v>4</v>
-      </c>
-      <c r="L16" s="10">
-        <v>0</v>
-      </c>
-      <c r="M16" s="10">
-        <v>4</v>
-      </c>
-      <c r="N16" s="10">
-        <v>4</v>
-      </c>
-      <c r="O16" s="10">
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="10">
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
+        <v>4</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
+      <c r="M16" s="9">
+        <v>4</v>
+      </c>
+      <c r="N16" s="9">
+        <v>4</v>
+      </c>
+      <c r="O16" s="9">
+        <v>0</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="9">
         <v>7</v>
       </c>
-      <c r="R16" s="10">
-        <v>0</v>
-      </c>
-      <c r="S16" s="10">
-        <v>3</v>
-      </c>
-      <c r="T16" s="10">
-        <v>4</v>
-      </c>
-      <c r="U16" s="10">
+      <c r="R16" s="9">
+        <v>0</v>
+      </c>
+      <c r="S16" s="9">
+        <v>3</v>
+      </c>
+      <c r="T16" s="9">
+        <v>4</v>
+      </c>
+      <c r="U16" s="9">
         <v>3</v>
       </c>
     </row>
@@ -6079,62 +6076,62 @@
       <c r="A17" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="11" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11" t="s">
+      <c r="G17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <v>27</v>
       </c>
-      <c r="J17" s="10">
-        <v>0</v>
-      </c>
-      <c r="K17" s="10">
-        <v>4</v>
-      </c>
-      <c r="L17" s="10">
-        <v>0</v>
-      </c>
-      <c r="M17" s="10">
-        <v>4</v>
-      </c>
-      <c r="N17" s="10">
-        <v>3</v>
-      </c>
-      <c r="O17" s="10">
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="10">
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>4</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>4</v>
+      </c>
+      <c r="N17" s="9">
+        <v>3</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0</v>
+      </c>
+      <c r="P17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="9">
         <v>6</v>
       </c>
-      <c r="R17" s="10">
-        <v>0</v>
-      </c>
-      <c r="S17" s="10">
-        <v>3</v>
-      </c>
-      <c r="T17" s="10">
-        <v>4</v>
-      </c>
-      <c r="U17" s="10">
+      <c r="R17" s="9">
+        <v>0</v>
+      </c>
+      <c r="S17" s="9">
+        <v>3</v>
+      </c>
+      <c r="T17" s="9">
+        <v>4</v>
+      </c>
+      <c r="U17" s="9">
         <v>3</v>
       </c>
     </row>
@@ -6142,62 +6139,62 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="11" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="11" t="s">
+      <c r="G18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <v>26</v>
       </c>
-      <c r="J18" s="10">
-        <v>0</v>
-      </c>
-      <c r="K18" s="10">
-        <v>4</v>
-      </c>
-      <c r="L18" s="10">
-        <v>0</v>
-      </c>
-      <c r="M18" s="10">
-        <v>4</v>
-      </c>
-      <c r="N18" s="10">
-        <v>4</v>
-      </c>
-      <c r="O18" s="10">
-        <v>0</v>
-      </c>
-      <c r="P18" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>4</v>
-      </c>
-      <c r="R18" s="10">
-        <v>0</v>
-      </c>
-      <c r="S18" s="10">
-        <v>3</v>
-      </c>
-      <c r="T18" s="10">
-        <v>4</v>
-      </c>
-      <c r="U18" s="10">
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>4</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>4</v>
+      </c>
+      <c r="N18" s="9">
+        <v>4</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>4</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0</v>
+      </c>
+      <c r="S18" s="9">
+        <v>3</v>
+      </c>
+      <c r="T18" s="9">
+        <v>4</v>
+      </c>
+      <c r="U18" s="9">
         <v>3</v>
       </c>
     </row>
@@ -6205,62 +6202,62 @@
       <c r="A19" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="11" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" s="14">
+      <c r="G19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="13">
         <v>25</v>
       </c>
-      <c r="J19" s="10">
-        <v>0</v>
-      </c>
-      <c r="K19" s="10">
-        <v>4</v>
-      </c>
-      <c r="L19" s="10">
-        <v>0</v>
-      </c>
-      <c r="M19" s="10">
-        <v>4</v>
-      </c>
-      <c r="N19" s="10">
-        <v>3</v>
-      </c>
-      <c r="O19" s="10">
-        <v>0</v>
-      </c>
-      <c r="P19" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="10">
-        <v>4</v>
-      </c>
-      <c r="R19" s="10">
-        <v>0</v>
-      </c>
-      <c r="S19" s="10">
-        <v>3</v>
-      </c>
-      <c r="T19" s="10">
-        <v>4</v>
-      </c>
-      <c r="U19" s="10">
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>4</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>4</v>
+      </c>
+      <c r="N19" s="9">
+        <v>3</v>
+      </c>
+      <c r="O19" s="9">
+        <v>0</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>4</v>
+      </c>
+      <c r="R19" s="9">
+        <v>0</v>
+      </c>
+      <c r="S19" s="9">
+        <v>3</v>
+      </c>
+      <c r="T19" s="9">
+        <v>4</v>
+      </c>
+      <c r="U19" s="9">
         <v>3</v>
       </c>
     </row>
@@ -6268,62 +6265,62 @@
       <c r="A20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="11" t="s">
+      <c r="G20" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <v>52</v>
       </c>
-      <c r="J20" s="10">
-        <v>0</v>
-      </c>
-      <c r="K20" s="10">
-        <v>0</v>
-      </c>
-      <c r="L20" s="10">
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0</v>
+      </c>
+      <c r="L20" s="9">
         <v>7</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>7</v>
       </c>
-      <c r="N20" s="10">
-        <v>4</v>
-      </c>
-      <c r="O20" s="10">
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="10">
+      <c r="N20" s="9">
+        <v>4</v>
+      </c>
+      <c r="O20" s="9">
+        <v>0</v>
+      </c>
+      <c r="P20" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="9">
         <v>9</v>
       </c>
-      <c r="R20" s="10">
-        <v>3</v>
-      </c>
-      <c r="S20" s="10">
+      <c r="R20" s="9">
+        <v>3</v>
+      </c>
+      <c r="S20" s="9">
         <v>7</v>
       </c>
-      <c r="T20" s="10">
+      <c r="T20" s="9">
         <v>6</v>
       </c>
-      <c r="U20" s="10">
+      <c r="U20" s="9">
         <v>6</v>
       </c>
     </row>
@@ -6331,62 +6328,62 @@
       <c r="A21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="11" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="11" t="s">
+      <c r="G21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="13">
         <v>50</v>
       </c>
-      <c r="J21" s="10">
-        <v>0</v>
-      </c>
-      <c r="K21" s="10">
-        <v>0</v>
-      </c>
-      <c r="L21" s="10">
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
         <v>7</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <v>7</v>
       </c>
-      <c r="N21" s="10">
-        <v>4</v>
-      </c>
-      <c r="O21" s="10">
-        <v>0</v>
-      </c>
-      <c r="P21" s="10">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="10">
+      <c r="N21" s="9">
+        <v>4</v>
+      </c>
+      <c r="O21" s="9">
+        <v>0</v>
+      </c>
+      <c r="P21" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="9">
         <v>7</v>
       </c>
-      <c r="R21" s="10">
-        <v>3</v>
-      </c>
-      <c r="S21" s="10">
+      <c r="R21" s="9">
+        <v>3</v>
+      </c>
+      <c r="S21" s="9">
         <v>7</v>
       </c>
-      <c r="T21" s="10">
+      <c r="T21" s="9">
         <v>6</v>
       </c>
-      <c r="U21" s="10">
+      <c r="U21" s="9">
         <v>6</v>
       </c>
     </row>
@@ -6394,62 +6391,62 @@
       <c r="A22" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="11" t="s">
+      <c r="E22" s="11"/>
+      <c r="F22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="G22" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="13">
         <v>52</v>
       </c>
-      <c r="J22" s="10">
-        <v>0</v>
-      </c>
-      <c r="K22" s="10">
-        <v>0</v>
-      </c>
-      <c r="L22" s="10">
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9">
         <v>7</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="9">
         <v>7</v>
       </c>
-      <c r="N22" s="10">
-        <v>4</v>
-      </c>
-      <c r="O22" s="10">
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="10">
+      <c r="N22" s="9">
+        <v>4</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0</v>
+      </c>
+      <c r="P22" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="9">
         <v>9</v>
       </c>
-      <c r="R22" s="10">
-        <v>3</v>
-      </c>
-      <c r="S22" s="10">
+      <c r="R22" s="9">
+        <v>3</v>
+      </c>
+      <c r="S22" s="9">
         <v>7</v>
       </c>
-      <c r="T22" s="10">
+      <c r="T22" s="9">
         <v>6</v>
       </c>
-      <c r="U22" s="10">
+      <c r="U22" s="9">
         <v>6</v>
       </c>
     </row>
@@ -6457,62 +6454,62 @@
       <c r="A23" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="11" t="s">
+      <c r="E23" s="11"/>
+      <c r="F23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="14">
+      <c r="G23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
         <v>50</v>
       </c>
-      <c r="J23" s="10">
-        <v>0</v>
-      </c>
-      <c r="K23" s="10">
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9">
         <v>7</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="9">
         <v>7</v>
       </c>
-      <c r="N23" s="10">
-        <v>4</v>
-      </c>
-      <c r="O23" s="10">
-        <v>0</v>
-      </c>
-      <c r="P23" s="10">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="10">
+      <c r="N23" s="9">
+        <v>4</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0</v>
+      </c>
+      <c r="P23" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="9">
         <v>7</v>
       </c>
-      <c r="R23" s="10">
-        <v>3</v>
-      </c>
-      <c r="S23" s="10">
+      <c r="R23" s="9">
+        <v>3</v>
+      </c>
+      <c r="S23" s="9">
         <v>7</v>
       </c>
-      <c r="T23" s="10">
+      <c r="T23" s="9">
         <v>6</v>
       </c>
-      <c r="U23" s="10">
+      <c r="U23" s="9">
         <v>6</v>
       </c>
     </row>
@@ -6520,62 +6517,62 @@
       <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="11" t="s">
+      <c r="E24" s="11"/>
+      <c r="F24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="11" t="s">
+      <c r="G24" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="13">
         <v>47</v>
       </c>
-      <c r="J24" s="10">
-        <v>0</v>
-      </c>
-      <c r="K24" s="10">
-        <v>0</v>
-      </c>
-      <c r="L24" s="10">
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0</v>
+      </c>
+      <c r="L24" s="9">
         <v>7</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="9">
         <v>7</v>
       </c>
-      <c r="N24" s="10">
-        <v>4</v>
-      </c>
-      <c r="O24" s="10">
-        <v>0</v>
-      </c>
-      <c r="P24" s="10">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="10">
+      <c r="N24" s="9">
+        <v>4</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0</v>
+      </c>
+      <c r="P24" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="9">
         <v>7</v>
       </c>
-      <c r="R24" s="10">
-        <v>3</v>
-      </c>
-      <c r="S24" s="10">
+      <c r="R24" s="9">
+        <v>3</v>
+      </c>
+      <c r="S24" s="9">
         <v>6</v>
       </c>
-      <c r="T24" s="10">
+      <c r="T24" s="9">
         <v>6</v>
       </c>
-      <c r="U24" s="10">
+      <c r="U24" s="9">
         <v>4</v>
       </c>
     </row>
@@ -6583,62 +6580,62 @@
       <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11" t="s">
+      <c r="E25" s="11"/>
+      <c r="F25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25" s="11" t="s">
+      <c r="G25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="13">
         <v>47</v>
       </c>
-      <c r="J25" s="10">
-        <v>0</v>
-      </c>
-      <c r="K25" s="10">
-        <v>0</v>
-      </c>
-      <c r="L25" s="10">
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
         <v>7</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="9">
         <v>7</v>
       </c>
-      <c r="N25" s="10">
-        <v>4</v>
-      </c>
-      <c r="O25" s="10">
-        <v>0</v>
-      </c>
-      <c r="P25" s="10">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="10">
+      <c r="N25" s="9">
+        <v>4</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0</v>
+      </c>
+      <c r="P25" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="9">
         <v>7</v>
       </c>
-      <c r="R25" s="10">
-        <v>3</v>
-      </c>
-      <c r="S25" s="10">
+      <c r="R25" s="9">
+        <v>3</v>
+      </c>
+      <c r="S25" s="9">
         <v>6</v>
       </c>
-      <c r="T25" s="10">
+      <c r="T25" s="9">
         <v>6</v>
       </c>
-      <c r="U25" s="10">
+      <c r="U25" s="9">
         <v>4</v>
       </c>
     </row>
@@ -6646,62 +6643,62 @@
       <c r="A26" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11" t="s">
+      <c r="E26" s="11"/>
+      <c r="F26" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26" s="11" t="s">
+      <c r="G26" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="14">
-        <v>3</v>
-      </c>
-      <c r="J26" s="10">
-        <v>0</v>
-      </c>
-      <c r="K26" s="10">
-        <v>0</v>
-      </c>
-      <c r="L26" s="10">
-        <v>0</v>
-      </c>
-      <c r="M26" s="10">
-        <v>0</v>
-      </c>
-      <c r="N26" s="10">
-        <v>0</v>
-      </c>
-      <c r="O26" s="10">
-        <v>0</v>
-      </c>
-      <c r="P26" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="10">
-        <v>3</v>
-      </c>
-      <c r="R26" s="10">
-        <v>0</v>
-      </c>
-      <c r="S26" s="10">
-        <v>0</v>
-      </c>
-      <c r="T26" s="10">
-        <v>0</v>
-      </c>
-      <c r="U26" s="10">
+      <c r="I26" s="13">
+        <v>3</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0</v>
+      </c>
+      <c r="N26" s="9">
+        <v>0</v>
+      </c>
+      <c r="O26" s="9">
+        <v>0</v>
+      </c>
+      <c r="P26" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>3</v>
+      </c>
+      <c r="R26" s="9">
+        <v>0</v>
+      </c>
+      <c r="S26" s="9">
+        <v>0</v>
+      </c>
+      <c r="T26" s="9">
+        <v>0</v>
+      </c>
+      <c r="U26" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6709,62 +6706,62 @@
       <c r="A27" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="11" t="s">
+      <c r="E27" s="11"/>
+      <c r="F27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="11" t="s">
+      <c r="G27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="14">
-        <v>3</v>
-      </c>
-      <c r="J27" s="10">
-        <v>0</v>
-      </c>
-      <c r="K27" s="10">
-        <v>0</v>
-      </c>
-      <c r="L27" s="10">
-        <v>0</v>
-      </c>
-      <c r="M27" s="10">
-        <v>0</v>
-      </c>
-      <c r="N27" s="10">
-        <v>0</v>
-      </c>
-      <c r="O27" s="10">
-        <v>0</v>
-      </c>
-      <c r="P27" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="10">
-        <v>3</v>
-      </c>
-      <c r="R27" s="10">
-        <v>0</v>
-      </c>
-      <c r="S27" s="10">
-        <v>0</v>
-      </c>
-      <c r="T27" s="10">
-        <v>0</v>
-      </c>
-      <c r="U27" s="10">
+      <c r="I27" s="13">
+        <v>3</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>0</v>
+      </c>
+      <c r="O27" s="9">
+        <v>0</v>
+      </c>
+      <c r="P27" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>3</v>
+      </c>
+      <c r="R27" s="9">
+        <v>0</v>
+      </c>
+      <c r="S27" s="9">
+        <v>0</v>
+      </c>
+      <c r="T27" s="9">
+        <v>0</v>
+      </c>
+      <c r="U27" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6772,62 +6769,62 @@
       <c r="A28" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="11" t="s">
+      <c r="E28" s="11"/>
+      <c r="F28" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H28" s="11" t="s">
+      <c r="G28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="14">
-        <v>3</v>
-      </c>
-      <c r="J28" s="10">
-        <v>0</v>
-      </c>
-      <c r="K28" s="10">
-        <v>3</v>
-      </c>
-      <c r="L28" s="10">
-        <v>0</v>
-      </c>
-      <c r="M28" s="10">
-        <v>0</v>
-      </c>
-      <c r="N28" s="10">
-        <v>0</v>
-      </c>
-      <c r="O28" s="10">
-        <v>0</v>
-      </c>
-      <c r="P28" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="10">
-        <v>0</v>
-      </c>
-      <c r="R28" s="10">
-        <v>0</v>
-      </c>
-      <c r="S28" s="10">
-        <v>0</v>
-      </c>
-      <c r="T28" s="10">
-        <v>0</v>
-      </c>
-      <c r="U28" s="10">
+      <c r="I28" s="13">
+        <v>3</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0</v>
+      </c>
+      <c r="K28" s="9">
+        <v>3</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0</v>
+      </c>
+      <c r="P28" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>0</v>
+      </c>
+      <c r="R28" s="9">
+        <v>0</v>
+      </c>
+      <c r="S28" s="9">
+        <v>0</v>
+      </c>
+      <c r="T28" s="9">
+        <v>0</v>
+      </c>
+      <c r="U28" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6835,62 +6832,62 @@
       <c r="A29" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="11" t="s">
+      <c r="E29" s="11"/>
+      <c r="F29" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="11" t="s">
+      <c r="G29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="14">
-        <v>3</v>
-      </c>
-      <c r="J29" s="10">
-        <v>0</v>
-      </c>
-      <c r="K29" s="10">
-        <v>3</v>
-      </c>
-      <c r="L29" s="10">
-        <v>0</v>
-      </c>
-      <c r="M29" s="10">
-        <v>0</v>
-      </c>
-      <c r="N29" s="10">
-        <v>0</v>
-      </c>
-      <c r="O29" s="10">
-        <v>0</v>
-      </c>
-      <c r="P29" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="10">
-        <v>0</v>
-      </c>
-      <c r="R29" s="10">
-        <v>0</v>
-      </c>
-      <c r="S29" s="10">
-        <v>0</v>
-      </c>
-      <c r="T29" s="10">
-        <v>0</v>
-      </c>
-      <c r="U29" s="10">
+      <c r="I29" s="13">
+        <v>3</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>3</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+      <c r="P29" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>0</v>
+      </c>
+      <c r="R29" s="9">
+        <v>0</v>
+      </c>
+      <c r="S29" s="9">
+        <v>0</v>
+      </c>
+      <c r="T29" s="9">
+        <v>0</v>
+      </c>
+      <c r="U29" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6898,62 +6895,62 @@
       <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11" t="s">
+      <c r="E30" s="11"/>
+      <c r="F30" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="11" t="s">
+      <c r="G30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="14">
-        <v>3</v>
-      </c>
-      <c r="J30" s="10">
-        <v>0</v>
-      </c>
-      <c r="K30" s="10">
-        <v>3</v>
-      </c>
-      <c r="L30" s="10">
-        <v>0</v>
-      </c>
-      <c r="M30" s="10">
-        <v>0</v>
-      </c>
-      <c r="N30" s="10">
-        <v>0</v>
-      </c>
-      <c r="O30" s="10">
-        <v>0</v>
-      </c>
-      <c r="P30" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="10">
-        <v>0</v>
-      </c>
-      <c r="R30" s="10">
-        <v>0</v>
-      </c>
-      <c r="S30" s="10">
-        <v>0</v>
-      </c>
-      <c r="T30" s="10">
-        <v>0</v>
-      </c>
-      <c r="U30" s="10">
+      <c r="I30" s="13">
+        <v>3</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+      <c r="K30" s="9">
+        <v>3</v>
+      </c>
+      <c r="L30" s="9">
+        <v>0</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0</v>
+      </c>
+      <c r="N30" s="9">
+        <v>0</v>
+      </c>
+      <c r="O30" s="9">
+        <v>0</v>
+      </c>
+      <c r="P30" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>0</v>
+      </c>
+      <c r="R30" s="9">
+        <v>0</v>
+      </c>
+      <c r="S30" s="9">
+        <v>0</v>
+      </c>
+      <c r="T30" s="9">
+        <v>0</v>
+      </c>
+      <c r="U30" s="9">
         <v>0</v>
       </c>
     </row>
@@ -6961,62 +6958,62 @@
       <c r="A31" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="11" t="s">
+      <c r="E31" s="11"/>
+      <c r="F31" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="14">
-        <v>3</v>
-      </c>
-      <c r="J31" s="10">
-        <v>0</v>
-      </c>
-      <c r="K31" s="10">
-        <v>3</v>
-      </c>
-      <c r="L31" s="10">
-        <v>0</v>
-      </c>
-      <c r="M31" s="10">
-        <v>0</v>
-      </c>
-      <c r="N31" s="10">
-        <v>0</v>
-      </c>
-      <c r="O31" s="10">
-        <v>0</v>
-      </c>
-      <c r="P31" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="10">
-        <v>0</v>
-      </c>
-      <c r="R31" s="10">
-        <v>0</v>
-      </c>
-      <c r="S31" s="10">
-        <v>0</v>
-      </c>
-      <c r="T31" s="10">
-        <v>0</v>
-      </c>
-      <c r="U31" s="10">
+      <c r="G31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="13">
+        <v>3</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="9">
+        <v>3</v>
+      </c>
+      <c r="L31" s="9">
+        <v>0</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0</v>
+      </c>
+      <c r="O31" s="9">
+        <v>0</v>
+      </c>
+      <c r="P31" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>0</v>
+      </c>
+      <c r="R31" s="9">
+        <v>0</v>
+      </c>
+      <c r="S31" s="9">
+        <v>0</v>
+      </c>
+      <c r="T31" s="9">
+        <v>0</v>
+      </c>
+      <c r="U31" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>